<commit_message>
reading scenario info from the excel file. removed usage of moment objects usage of generic waypoint and tip names
</commit_message>
<xml_diff>
--- a/Senaryo.xlsx
+++ b/Senaryo.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="15570" windowHeight="9330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="15570" windowHeight="9330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SENARYO 1" sheetId="1" r:id="rId1"/>
@@ -461,15 +461,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -479,6 +470,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -749,7 +749,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -769,18 +769,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:12" s="5" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -818,7 +818,7 @@
       <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>82</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -853,7 +853,7 @@
       <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="12" t="s">
         <v>82</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -892,7 +892,7 @@
       <c r="A5" s="6">
         <v>3</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -927,7 +927,7 @@
       <c r="A6" s="6">
         <v>4</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="12" t="s">
         <v>82</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -962,7 +962,7 @@
       <c r="A7" s="6">
         <v>5</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="12" t="s">
         <v>82</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -997,7 +997,7 @@
       <c r="A8" s="6">
         <v>6</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="12" t="s">
         <v>82</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -1032,7 +1032,7 @@
       <c r="A9" s="6">
         <v>7</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
         <v>82</v>
       </c>
       <c r="C9" s="11" t="s">
@@ -1067,7 +1067,7 @@
       <c r="A10" s="6">
         <v>8</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -1102,7 +1102,7 @@
       <c r="A11" s="6">
         <v>9</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="12" t="s">
         <v>82</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -1137,7 +1137,7 @@
       <c r="A12" s="7">
         <v>10</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C12" s="11" t="s">
@@ -1211,7 +1211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1244,26 +1244,26 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="13">
         <f>B2+60</f>
         <v>425</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="13">
         <f t="shared" ref="D2:G2" si="0">C2+60</f>
         <v>485</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="13">
         <f t="shared" si="0"/>
         <v>545</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="13">
         <f t="shared" si="0"/>
         <v>605</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="13">
         <f t="shared" si="0"/>
         <v>665</v>
       </c>
@@ -1272,27 +1272,27 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="15">
         <f>7*60+29</f>
         <v>449</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="13">
         <f>B3+60</f>
         <v>509</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="13">
         <f t="shared" ref="D3:G3" si="1">C3+60</f>
         <v>569</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="13">
         <f t="shared" si="1"/>
         <v>629</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="13">
         <f t="shared" si="1"/>
         <v>689</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="13">
         <f t="shared" si="1"/>
         <v>749</v>
       </c>
@@ -1380,19 +1380,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
-      <c r="B1">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>300</v>
       </c>
     </row>

</xml_diff>